<commit_message>
statistics and results done
</commit_message>
<xml_diff>
--- a/TD_TO_frames.xlsx
+++ b/TD_TO_frames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Gangbild_Identitaet\Daten\Videos_Gait_ID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_David_Files\forensic\gait_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A2408E-6AAC-4522-AC5F-43DD149EDCF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791374AF-3A10-40ED-87B3-7AA49FB4B7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="960" windowWidth="24240" windowHeight="13020" xr2:uid="{28C826A1-F80E-4205-B29D-5D2A7264603C}"/>
   </bookViews>
@@ -735,7 +735,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -825,8 +825,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1141,21 +1141,23 @@
   <dimension ref="A1:P163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K138" sqref="K138:L139"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="12" width="13.5703125" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="12" width="13.5703125" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1235,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>6645</v>
       </c>
@@ -1269,7 +1271,7 @@
       </c>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>8050</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1340,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3595</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4298</v>
       </c>
@@ -1408,7 +1410,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1442,7 +1444,7 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>6148</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>7558</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="5" customFormat="1">
+    <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>4862</v>
       </c>
@@ -1585,7 +1587,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>6556</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>2736</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>3595</v>
       </c>
@@ -1728,7 +1730,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1766,7 +1768,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>4297</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>6003</v>
       </c>
@@ -1836,7 +1838,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="5" customFormat="1">
+    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1870,7 +1872,7 @@
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>6056</v>
       </c>
@@ -1901,7 +1903,7 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>10167</v>
       </c>
@@ -1932,7 +1934,7 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1966,7 +1968,7 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>2981</v>
       </c>
@@ -1997,7 +1999,7 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>5031</v>
       </c>
@@ -2028,7 +2030,7 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2056,13 +2058,10 @@
       <c r="I26">
         <v>207</v>
       </c>
-      <c r="J26">
-        <v>204</v>
-      </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>6346</v>
       </c>
@@ -2093,7 +2092,7 @@
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>10456</v>
       </c>
@@ -2125,7 +2124,7 @@
       <c r="L28" s="10"/>
       <c r="P28" s="9"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -2160,7 +2159,7 @@
       <c r="L29" s="10"/>
       <c r="P29" s="9"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>5826</v>
       </c>
@@ -2191,7 +2190,7 @@
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>9925</v>
       </c>
@@ -2222,7 +2221,7 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
     </row>
-    <row r="32" spans="1:16" s="5" customFormat="1">
+    <row r="32" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>54</v>
       </c>
@@ -2260,7 +2259,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>18866</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>22050</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2368,7 +2367,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>9627</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>11225</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <v>18747</v>
       </c>
@@ -2511,7 +2510,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>21935</v>
       </c>
@@ -2546,7 +2545,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" s="3">
         <v>9958</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>13153</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="5" customFormat="1">
+    <row r="44" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>70</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>7756</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>11196</v>
       </c>
@@ -2762,7 +2761,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -2800,7 +2799,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
         <v>3973</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49" s="3">
         <v>5688</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>78</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>7661</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>11102</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>7567</v>
       </c>
@@ -3051,7 +3050,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="3">
         <v>10996</v>
       </c>
@@ -3086,7 +3085,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="5" customFormat="1">
+    <row r="56" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>86</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
         <v>7005</v>
       </c>
@@ -3159,7 +3158,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>10107</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>3442</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>4999</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B63" s="3">
         <v>6709</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" s="3">
         <v>9813</v>
       </c>
@@ -3410,7 +3409,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>98</v>
       </c>
@@ -3448,7 +3447,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>6584</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B67" s="3">
         <v>9700</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="5" customFormat="1">
+    <row r="68" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>102</v>
       </c>
@@ -3556,7 +3555,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>5777</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B70" s="3">
         <v>7053</v>
       </c>
@@ -3626,7 +3625,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B72" s="4">
         <v>2943</v>
       </c>
@@ -3699,7 +3698,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>3588</v>
       </c>
@@ -3734,7 +3733,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>110</v>
       </c>
@@ -3772,7 +3771,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B75" s="3">
         <v>6000</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" s="3">
         <v>7271</v>
       </c>
@@ -3842,7 +3841,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>114</v>
       </c>
@@ -3880,7 +3879,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="3">
         <v>6111</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="79" spans="1:12" s="7" customFormat="1">
+    <row r="79" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="8">
         <v>7387</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>118</v>
       </c>
@@ -3988,7 +3987,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B81" s="3">
         <v>6419</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82" s="3">
         <v>10568</v>
       </c>
@@ -4058,7 +4057,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>122</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B84" s="3">
         <v>6267</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B85" s="3">
         <v>10437</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>126</v>
       </c>
@@ -4204,7 +4203,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B87" s="3">
         <v>6364</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B88" s="3">
         <v>10511</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>130</v>
       </c>
@@ -4312,7 +4311,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>3754</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" spans="1:12" s="7" customFormat="1">
+    <row r="91" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="7">
         <v>5829</v>
       </c>
@@ -4382,7 +4381,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>134</v>
       </c>
@@ -4420,7 +4419,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B93" s="3">
         <v>4830</v>
       </c>
@@ -4455,7 +4454,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B94" s="3">
         <v>8987</v>
       </c>
@@ -4490,7 +4489,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>138</v>
       </c>
@@ -4528,7 +4527,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B96" s="3">
         <v>5063</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B97" s="3">
         <v>9231</v>
       </c>
@@ -4598,7 +4597,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>142</v>
       </c>
@@ -4636,7 +4635,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B99" s="3">
         <v>4963</v>
       </c>
@@ -4671,7 +4670,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B100" s="3">
         <v>9127</v>
       </c>
@@ -4706,7 +4705,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -4744,7 +4743,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B102" s="3">
         <v>1724</v>
       </c>
@@ -4779,7 +4778,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="1:12" s="7" customFormat="1">
+    <row r="103" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="8">
         <v>3806</v>
       </c>
@@ -4814,7 +4813,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B105" s="3">
         <v>4328</v>
       </c>
@@ -4887,7 +4886,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B106" s="3">
         <v>6998</v>
       </c>
@@ -4922,7 +4921,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>154</v>
       </c>
@@ -4960,7 +4959,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B108" s="3">
         <v>3999</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B109" s="3">
         <v>6657</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>158</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B111" s="3">
         <v>4113</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B112" s="3">
         <v>6777</v>
       </c>
@@ -5138,7 +5137,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>162</v>
       </c>
@@ -5176,7 +5175,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>2222</v>
       </c>
@@ -5211,7 +5210,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="115" spans="1:12" s="7" customFormat="1">
+    <row r="115" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="7">
         <v>3552</v>
       </c>
@@ -5246,7 +5245,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>166</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B117" s="3">
         <v>10182</v>
       </c>
@@ -5319,7 +5318,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B118" s="3">
         <v>11468</v>
       </c>
@@ -5354,7 +5353,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>170</v>
       </c>
@@ -5392,7 +5391,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B120" s="3">
         <v>10404</v>
       </c>
@@ -5427,7 +5426,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B121" s="3">
         <v>11692</v>
       </c>
@@ -5462,7 +5461,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>174</v>
       </c>
@@ -5500,7 +5499,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123" s="3">
         <v>10299</v>
       </c>
@@ -5535,7 +5534,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124" s="3">
         <v>11574</v>
       </c>
@@ -5570,7 +5569,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>178</v>
       </c>
@@ -5608,7 +5607,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126" s="3">
         <v>4384</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="127" spans="1:12" s="7" customFormat="1">
+    <row r="127" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="8">
         <v>5022</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>182</v>
       </c>
@@ -5716,7 +5715,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B129" s="3">
         <v>3543</v>
       </c>
@@ -5747,7 +5746,7 @@
       <c r="K129" s="10"/>
       <c r="L129" s="10"/>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B130" s="3">
         <v>4940</v>
       </c>
@@ -5778,7 +5777,7 @@
       <c r="K130" s="10"/>
       <c r="L130" s="10"/>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>186</v>
       </c>
@@ -5816,7 +5815,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B132" s="3">
         <v>3384</v>
       </c>
@@ -5847,7 +5846,7 @@
       <c r="K132" s="10"/>
       <c r="L132" s="10"/>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B133" s="3">
         <v>4777</v>
       </c>
@@ -5878,7 +5877,7 @@
       <c r="K133" s="10"/>
       <c r="L133" s="10"/>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>190</v>
       </c>
@@ -5916,7 +5915,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B135" s="3">
         <v>3469</v>
       </c>
@@ -5947,7 +5946,7 @@
       <c r="K135" s="10"/>
       <c r="L135" s="10"/>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B136" s="3">
         <v>4864</v>
       </c>
@@ -5978,7 +5977,7 @@
       <c r="K136" s="10"/>
       <c r="L136" s="10"/>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>194</v>
       </c>
@@ -6016,7 +6015,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>1833</v>
       </c>
@@ -6047,7 +6046,7 @@
       <c r="K138" s="10"/>
       <c r="L138" s="10"/>
     </row>
-    <row r="139" spans="1:12" s="7" customFormat="1">
+    <row r="139" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="7">
         <v>2537</v>
       </c>
@@ -6078,7 +6077,7 @@
       <c r="K139" s="12"/>
       <c r="L139" s="12"/>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>198</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B141" s="3">
         <v>5392</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B142" s="3">
         <v>6708</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -6224,7 +6223,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B144" s="3">
         <v>5129</v>
       </c>
@@ -6259,7 +6258,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B145" s="3">
         <v>6426</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>206</v>
       </c>
@@ -6332,7 +6331,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B147" s="3">
         <v>5216</v>
       </c>
@@ -6367,7 +6366,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B148" s="3">
         <v>6539</v>
       </c>
@@ -6402,7 +6401,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>210</v>
       </c>
@@ -6440,7 +6439,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B150" s="3">
         <v>2760</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:12" s="7" customFormat="1">
+    <row r="151" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B151" s="8">
         <v>3410</v>
       </c>
@@ -6510,7 +6509,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>214</v>
       </c>
@@ -6548,7 +6547,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B153" s="3">
         <v>5379</v>
       </c>
@@ -6583,7 +6582,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B154" s="3">
         <v>6789</v>
       </c>
@@ -6618,7 +6617,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>218</v>
       </c>
@@ -6656,7 +6655,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B156" s="3">
         <v>5235</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="157" spans="1:12">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B157" s="3">
         <v>6651</v>
       </c>
@@ -6726,7 +6725,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="158" spans="1:12">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>222</v>
       </c>
@@ -6764,7 +6763,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="159" spans="1:12">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B159" s="3">
         <v>5319</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B160" s="3">
         <v>6736</v>
       </c>
@@ -6815,9 +6814,6 @@
       <c r="F160">
         <v>110</v>
       </c>
-      <c r="G160">
-        <v>132</v>
-      </c>
       <c r="H160">
         <v>168</v>
       </c>
@@ -6834,7 +6830,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="161" spans="1:12">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>226</v>
       </c>
@@ -6872,7 +6868,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="1:12">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B162" s="3">
         <v>2750</v>
       </c>
@@ -6907,7 +6903,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B163" s="3">
         <v>3456</v>
       </c>

</xml_diff>